<commit_message>
Ran a test that opens a link in the browser.
</commit_message>
<xml_diff>
--- a/cli-data.xlsx
+++ b/cli-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miket/Downloads/Portfolio_Projects/cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1F9F8EE-90DE-F246-81F9-DC5E6A18C317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB1AAF6-E5D6-1845-BF2D-EC248E7995FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8380" yWindow="3600" windowWidth="28040" windowHeight="17440" xr2:uid="{6CA73D46-76A3-A741-B3B0-A36E9DABD96B}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>https://www.google.com</t>
+  </si>
+  <si>
+    <t>https://www.hostpapa.com</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C92B58C-CFEA-E04A-BA09-4F80A809864D}">
-  <dimension ref="B7"/>
+  <dimension ref="B7:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,9 +437,15 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{2BD0EF77-4482-1644-BBC1-666CDA21F4A5}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{F68CCE4C-59DB-E748-8DA0-4A51A2D45647}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Initial task of comparing data between xlsx files.
</commit_message>
<xml_diff>
--- a/cli-data.xlsx
+++ b/cli-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miket/Downloads/Portfolio_Projects/cli/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB1AAF6-E5D6-1845-BF2D-EC248E7995FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01136915-58E3-1C4E-A553-D5AEBC6BF934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8380" yWindow="3600" windowWidth="28040" windowHeight="17440" xr2:uid="{6CA73D46-76A3-A741-B3B0-A36E9DABD96B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <t>https://www.google.com</t>
   </si>
   <si>
-    <t>https://www.hostpapa.com</t>
+    <t>https://www.leetcode.com</t>
   </si>
 </sst>
 </file>
@@ -427,7 +427,7 @@
   <dimension ref="B7:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>